<commit_message>
added some ditails in TestCase.xlsx
</commit_message>
<xml_diff>
--- a/test_case/TestCase.xlsx
+++ b/test_case/TestCase.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MacBook Air\Desktop\gitTest2\SecondRepository\test_case\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MacBook Air\Desktop\ДЗ9\test_case\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF8AF4B0-5245-4E95-BDD3-B0247D9F347D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{782D51CE-E8C8-43FB-9465-24E48E68F203}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{971196F4-FD47-43E0-B842-C630B3DE48C1}"/>
   </bookViews>
@@ -57,9 +57,6 @@
     <t>Failed</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Открылся сайт                                                                   2. Открылась форма "Управление профилем"                              3. Форма редактирования стала активна для изменений                                                                               4. Введен новый номер телефона  "+79501908463" и отображается на экране                                                                                                  5. Кнопка "Получить код" сработала                            6. Пришел "SMS код" на новый номер телефона                                                                                              </t>
-  </si>
-  <si>
     <t>Наличие в профиле уже существующего зарегистрированого номера телефона</t>
   </si>
   <si>
@@ -69,10 +66,13 @@
     <t>Сменяемость уже существующего номера телефона на новые значения, с получение "SMS кода" на новый номер телефона</t>
   </si>
   <si>
-    <t xml:space="preserve">Управление профилем, смена существующего номера телефона на новый и получение "SMS код"на новый номер телефона при нажатие на кнопку "Получить  код" </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Открыть сайт                                                                      2.  Открыть форму "Управление профилем"                                                                                3. Кликнуть на кнопку "Редактировать"                                           4. Ввести в поле номера телефона вместо существующего новый номер                                       "+79501908463"                                                                       5. Кликнуть на кнопку "Получить код"                                          6. Проверить новый номер телефона на наличие "SMS кода"                                                                                 </t>
+    <t xml:space="preserve">Управление профилем, смена существующего номера телефона на новый и получение "SMS код" на новый номер телефона при нажатие на кнопку "Получить  код" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Открыть сайт                                                                      2.  Открыть форму "Управление профилем"                                                                                3. Кликнуть на кнопку "Редактировать"                                           4. Ввести в поле номера телефона вместо существующего новый номер                                       "+79501908463"                                                                       5. Кликнуть на кнопку "Получить код"                                          6. Проверить новый номер телефона на наличие "SMS кода"                                                                                7. Ввести пришедший "SMS кода"  в поле "SMS кода"                                                                                           8.  Кликнуть на кнопку "Подтвердить коды"                                                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Открылся сайт                                                                   2. Открылась форма "Управление профилем"                              3. Форма редактирования стала активна для изменений                                                                               4. Введен новый номер телефона  "+79501908463" и отображается на экране                                                                                                  5. Кнопка "Получить код" сработала                            6. Пришел "SMS код" на новый номер телефона   7. Введен "SMS код" в поле "SMS код"                       8. Замена номера прошла успешно                                                                                             </t>
   </si>
 </sst>
 </file>
@@ -286,6 +286,51 @@
   </cellStyleXfs>
   <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -295,50 +340,59 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -372,60 +426,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -777,293 +777,293 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="4" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="4" t="s">
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="6"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="12"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="39" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="39" t="s">
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="21"/>
+    </row>
+    <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="24"/>
+    </row>
+    <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="24"/>
+    </row>
+    <row r="5" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="22"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="24"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="24"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="22"/>
+      <c r="N6" s="23"/>
+      <c r="O6" s="23"/>
+      <c r="P6" s="23"/>
+      <c r="Q6" s="24"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="42"/>
+      <c r="B7" s="43"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="22"/>
+      <c r="N7" s="23"/>
+      <c r="O7" s="23"/>
+      <c r="P7" s="23"/>
+      <c r="Q7" s="24"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="42"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="23"/>
+      <c r="O8" s="23"/>
+      <c r="P8" s="23"/>
+      <c r="Q8" s="24"/>
+    </row>
+    <row r="9" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="45"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="23"/>
+      <c r="O9" s="23"/>
+      <c r="P9" s="23"/>
+      <c r="Q9" s="24"/>
+    </row>
+    <row r="10" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="23"/>
+      <c r="O10" s="23"/>
+      <c r="P10" s="23"/>
+      <c r="Q10" s="24"/>
+    </row>
+    <row r="11" spans="1:17" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="27"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="25"/>
+      <c r="N11" s="26"/>
+      <c r="O11" s="26"/>
+      <c r="P11" s="26"/>
+      <c r="Q11" s="27"/>
+    </row>
+    <row r="12" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-      <c r="P2" s="40"/>
-      <c r="Q2" s="41"/>
-    </row>
-    <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="42"/>
-      <c r="N3" s="43"/>
-      <c r="O3" s="43"/>
-      <c r="P3" s="43"/>
-      <c r="Q3" s="44"/>
-    </row>
-    <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="16"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="43"/>
-      <c r="K4" s="44"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="42"/>
-      <c r="N4" s="43"/>
-      <c r="O4" s="43"/>
-      <c r="P4" s="43"/>
-      <c r="Q4" s="44"/>
-    </row>
-    <row r="5" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="43"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="43"/>
-      <c r="K5" s="44"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="42"/>
-      <c r="N5" s="43"/>
-      <c r="O5" s="43"/>
-      <c r="P5" s="43"/>
-      <c r="Q5" s="44"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="44"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="42"/>
-      <c r="N6" s="43"/>
-      <c r="O6" s="43"/>
-      <c r="P6" s="43"/>
-      <c r="Q6" s="44"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="43"/>
-      <c r="K7" s="44"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="42"/>
-      <c r="N7" s="43"/>
-      <c r="O7" s="43"/>
-      <c r="P7" s="43"/>
-      <c r="Q7" s="44"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="24"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="43"/>
-      <c r="K8" s="44"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="42"/>
-      <c r="N8" s="43"/>
-      <c r="O8" s="43"/>
-      <c r="P8" s="43"/>
-      <c r="Q8" s="44"/>
-    </row>
-    <row r="9" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="27"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
-      <c r="J9" s="43"/>
-      <c r="K9" s="44"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="42"/>
-      <c r="N9" s="43"/>
-      <c r="O9" s="43"/>
-      <c r="P9" s="43"/>
-      <c r="Q9" s="44"/>
-    </row>
-    <row r="10" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="16"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
-      <c r="J10" s="43"/>
-      <c r="K10" s="44"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="42"/>
-      <c r="N10" s="43"/>
-      <c r="O10" s="43"/>
-      <c r="P10" s="43"/>
-      <c r="Q10" s="44"/>
-    </row>
-    <row r="11" spans="1:17" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="45"/>
-      <c r="H11" s="46"/>
-      <c r="I11" s="46"/>
-      <c r="J11" s="46"/>
-      <c r="K11" s="47"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="45"/>
-      <c r="N11" s="46"/>
-      <c r="O11" s="46"/>
-      <c r="P11" s="46"/>
-      <c r="Q11" s="47"/>
-    </row>
-    <row r="12" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="21" t="s">
+      <c r="B12" s="40"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="9"/>
+    </row>
+    <row r="13" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="42"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="12"/>
+    </row>
+    <row r="14" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="45"/>
+      <c r="B14" s="46"/>
+      <c r="C14" s="46"/>
+      <c r="D14" s="46"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="48" t="s">
         <v>11</v>
-      </c>
-      <c r="B12" s="22"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="16"/>
-      <c r="N12" s="17"/>
-      <c r="O12" s="17"/>
-      <c r="P12" s="17"/>
-      <c r="Q12" s="18"/>
-    </row>
-    <row r="13" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="24"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
-      <c r="P13" s="5"/>
-      <c r="Q13" s="6"/>
-    </row>
-    <row r="14" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="27"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="H14" s="31"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="31"/>
-      <c r="K14" s="32"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="48" t="s">
-        <v>12</v>
       </c>
       <c r="N14" s="49"/>
       <c r="O14" s="49"/>
@@ -1071,18 +1071,18 @@
       <c r="Q14" s="50"/>
     </row>
     <row r="15" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="16"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="35"/>
-      <c r="L15" s="2"/>
+      <c r="A15" s="7"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="33"/>
+      <c r="L15" s="17"/>
       <c r="M15" s="51"/>
       <c r="N15" s="52"/>
       <c r="O15" s="52"/>
@@ -1090,20 +1090,20 @@
       <c r="Q15" s="53"/>
     </row>
     <row r="16" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="34"/>
-      <c r="K16" s="35"/>
-      <c r="L16" s="2"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="32"/>
+      <c r="J16" s="32"/>
+      <c r="K16" s="33"/>
+      <c r="L16" s="17"/>
       <c r="M16" s="51"/>
       <c r="N16" s="52"/>
       <c r="O16" s="52"/>
@@ -1111,20 +1111,20 @@
       <c r="Q16" s="53"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="34"/>
-      <c r="I17" s="34"/>
-      <c r="J17" s="34"/>
-      <c r="K17" s="35"/>
-      <c r="L17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="33"/>
+      <c r="L17" s="17"/>
       <c r="M17" s="51"/>
       <c r="N17" s="52"/>
       <c r="O17" s="52"/>
@@ -1132,18 +1132,18 @@
       <c r="Q17" s="53"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="34"/>
-      <c r="J18" s="34"/>
-      <c r="K18" s="35"/>
-      <c r="L18" s="2"/>
+      <c r="A18" s="13"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="32"/>
+      <c r="J18" s="32"/>
+      <c r="K18" s="33"/>
+      <c r="L18" s="17"/>
       <c r="M18" s="51"/>
       <c r="N18" s="52"/>
       <c r="O18" s="52"/>
@@ -1151,18 +1151,18 @@
       <c r="Q18" s="53"/>
     </row>
     <row r="19" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="13"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
-      <c r="K19" s="38"/>
-      <c r="L19" s="3"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="35"/>
+      <c r="J19" s="35"/>
+      <c r="K19" s="36"/>
+      <c r="L19" s="18"/>
       <c r="M19" s="54"/>
       <c r="N19" s="55"/>
       <c r="O19" s="55"/>
@@ -1171,16 +1171,22 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="L1:L19"/>
+    <mergeCell ref="M1:Q1"/>
+    <mergeCell ref="M2:Q11"/>
+    <mergeCell ref="M12:Q12"/>
+    <mergeCell ref="M13:Q13"/>
+    <mergeCell ref="M14:Q19"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="G2:K11"/>
+    <mergeCell ref="G12:K12"/>
+    <mergeCell ref="G13:K13"/>
+    <mergeCell ref="G14:K19"/>
     <mergeCell ref="A2:E3"/>
     <mergeCell ref="A15:E15"/>
     <mergeCell ref="A16:E16"/>
     <mergeCell ref="A17:E19"/>
     <mergeCell ref="F1:F19"/>
-    <mergeCell ref="G1:K1"/>
-    <mergeCell ref="G2:K11"/>
-    <mergeCell ref="G12:K12"/>
-    <mergeCell ref="G13:K13"/>
-    <mergeCell ref="G14:K19"/>
     <mergeCell ref="A4:E4"/>
     <mergeCell ref="A5:E5"/>
     <mergeCell ref="A6:E9"/>
@@ -1188,12 +1194,6 @@
     <mergeCell ref="A11:E11"/>
     <mergeCell ref="A12:E14"/>
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="L1:L19"/>
-    <mergeCell ref="M1:Q1"/>
-    <mergeCell ref="M2:Q11"/>
-    <mergeCell ref="M12:Q12"/>
-    <mergeCell ref="M13:Q13"/>
-    <mergeCell ref="M14:Q19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>